<commit_message>
1. Add the remark command. 2. Fix the log1, log2 issue. 3. Add the remote control record function from merge trunk source.
</commit_message>
<xml_diff>
--- a/branches/Customer_Spider/AutoTest/AutoTest/bin/Debug/Schedule/Script Template.xlsx
+++ b/branches/Customer_Spider/AutoTest/AutoTest/bin/Debug/Schedule/Script Template.xlsx
@@ -39,6 +39,7 @@
     <definedName name="_PB07_0">'Selection List'!$J$2:$J$9</definedName>
     <definedName name="_PB07_1">'Selection List'!$J$2:$J$9</definedName>
     <definedName name="_pwm">'Selection List'!$L$2:$L$102</definedName>
+    <definedName name="_SXP">'Selection List'!$I$2</definedName>
     <definedName name="AC_On_Off">'Selection List'!$E$2:$E$11</definedName>
     <definedName name="AC_Power_On_Off__Command">'Selection List'!$E$2:$E$11</definedName>
     <definedName name="Blank">'Selection List'!$I$2</definedName>
@@ -50,7 +51,7 @@
     <definedName name="PWM">'Selection List'!$L$2:$L$103</definedName>
     <definedName name="Quantum_color_space_Command">'Selection List'!$G$2:$G$10</definedName>
     <definedName name="Quantum_timing_Command">'Selection List'!$F$2:$F$105</definedName>
-    <definedName name="RC_Key">'Selection List'!$A$2:$A$114</definedName>
+    <definedName name="RC_Key">'Selection List'!$A$2:$A$116</definedName>
     <definedName name="Record_A_V_Command">'Selection List'!$C$2:$C$3</definedName>
     <definedName name="Timing_Command">'Selection List'!$F$2:$F$105</definedName>
   </definedNames>
@@ -79,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="283">
   <si>
     <t xml:space="preserve">RC Key </t>
   </si>
@@ -1039,59 +1040,26 @@
   </si>
   <si>
     <t>_pwm</t>
-  </si>
-  <si>
-    <t>_pwm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_log1</t>
-  </si>
-  <si>
-    <t>_clear</t>
-  </si>
-  <si>
-    <t>_log2</t>
-  </si>
-  <si>
-    <t>_save</t>
-  </si>
-  <si>
-    <t>_PA10_0</t>
-  </si>
-  <si>
-    <t>_rc_</t>
-  </si>
-  <si>
-    <t>_PB01_1</t>
-  </si>
-  <si>
-    <t>_logcmd</t>
-  </si>
-  <si>
-    <t>_audio_debounce</t>
-  </si>
-  <si>
-    <t>1000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_stop</t>
-  </si>
-  <si>
-    <t>_cmd</t>
-  </si>
-  <si>
-    <t>_shot</t>
-  </si>
-  <si>
-    <t>_quantum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>off</t>
-  </si>
-  <si>
-    <t>off</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_hex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DO NOT ADD ANY COMMA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_SXP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1144,7 +1112,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1220,6 +1188,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1303,7 +1277,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1418,11 +1392,64 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="33">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2996,21 +3023,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表格1" displayName="表格1" ref="A2:J26" headerRowCount="0" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表格1" displayName="表格1" ref="A2:K26" headerRowCount="0" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23" totalsRowBorderDxfId="22">
   <sortState ref="A3:J22">
     <sortCondition ref="H1:H22"/>
   </sortState>
-  <tableColumns count="10">
-    <tableColumn id="1" name="欄1" headerRowDxfId="19" dataDxfId="18"/>
-    <tableColumn id="2" name="欄2" headerRowDxfId="17" dataDxfId="16"/>
-    <tableColumn id="3" name="欄3" headerRowDxfId="15" dataDxfId="14"/>
-    <tableColumn id="4" name="欄4" headerRowDxfId="13" dataDxfId="12"/>
-    <tableColumn id="5" name="欄5" headerRowDxfId="11" dataDxfId="10"/>
-    <tableColumn id="6" name="欄6" headerRowDxfId="9" dataDxfId="8"/>
-    <tableColumn id="7" name="欄7" headerRowDxfId="7" dataDxfId="6"/>
-    <tableColumn id="11" name="欄8" headerRowDxfId="5" dataDxfId="4"/>
-    <tableColumn id="10" name="欄9" headerRowDxfId="3" dataDxfId="2"/>
-    <tableColumn id="8" name="欄10" headerRowDxfId="1" dataDxfId="0"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="欄1" headerRowDxfId="21" dataDxfId="20"/>
+    <tableColumn id="2" name="欄2" headerRowDxfId="19" dataDxfId="18"/>
+    <tableColumn id="3" name="欄3" headerRowDxfId="17" dataDxfId="16"/>
+    <tableColumn id="4" name="欄4" headerRowDxfId="15" dataDxfId="14"/>
+    <tableColumn id="5" name="欄5" headerRowDxfId="13" dataDxfId="12"/>
+    <tableColumn id="6" name="欄6" headerRowDxfId="11" dataDxfId="10"/>
+    <tableColumn id="7" name="欄7" headerRowDxfId="9" dataDxfId="8"/>
+    <tableColumn id="11" name="欄8" headerRowDxfId="7" dataDxfId="6"/>
+    <tableColumn id="10" name="欄9" headerRowDxfId="5" dataDxfId="4"/>
+    <tableColumn id="8" name="欄10" headerRowDxfId="3" dataDxfId="2"/>
+    <tableColumn id="9" name="欄11" headerRowDxfId="1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3303,28 +3331,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5" style="18" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="11.875" style="18" customWidth="1"/>
-    <col min="5" max="5" width="14.875" style="18" customWidth="1"/>
+    <col min="5" max="5" width="15" style="18" customWidth="1"/>
     <col min="6" max="6" width="11.875" style="18" customWidth="1"/>
     <col min="7" max="7" width="17" style="18" customWidth="1"/>
-    <col min="8" max="8" width="10.125" style="18" customWidth="1"/>
+    <col min="8" max="8" width="9.375" style="18" customWidth="1"/>
     <col min="9" max="9" width="16.75" style="18" customWidth="1"/>
     <col min="10" max="10" width="9.125" style="18" customWidth="1"/>
-    <col min="11" max="11" width="13.25" style="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.875" style="18" customWidth="1"/>
     <col min="12" max="12" width="13" style="18" customWidth="1"/>
     <col min="13" max="16384" width="9" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>210</v>
       </c>
@@ -3355,184 +3383,157 @@
       <c r="J1" s="16" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>279</v>
-      </c>
+      <c r="K1" s="39" t="s">
+        <v>280</v>
+      </c>
+      <c r="L1" s="18"/>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
       <c r="B2" s="25"/>
       <c r="C2" s="4"/>
       <c r="D2" s="5"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="25" t="s">
-        <v>280</v>
-      </c>
+      <c r="F2" s="25"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
-      <c r="J2" s="5"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="J2" s="38"/>
+      <c r="K2" s="40" t="s">
         <v>281</v>
       </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
       <c r="B3" s="25"/>
       <c r="C3" s="4"/>
       <c r="D3" s="5"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="25" t="s">
-        <v>282</v>
-      </c>
+      <c r="F3" s="25"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="29"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>283</v>
-      </c>
+      <c r="K3" s="40"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
       <c r="B4" s="25"/>
       <c r="C4" s="4"/>
       <c r="D4" s="5"/>
       <c r="E4" s="26"/>
-      <c r="F4" s="25" t="s">
-        <v>284</v>
-      </c>
+      <c r="F4" s="25"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="27"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>285</v>
-      </c>
+      <c r="K4" s="40"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
       <c r="B5" s="25"/>
       <c r="C5" s="4"/>
       <c r="D5" s="5"/>
       <c r="E5" s="26"/>
-      <c r="F5" s="25" t="s">
-        <v>286</v>
-      </c>
+      <c r="F5" s="25"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="27"/>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>287</v>
-      </c>
+      <c r="K5" s="40"/>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
       <c r="B6" s="25"/>
       <c r="C6" s="4"/>
       <c r="D6" s="5"/>
       <c r="E6" s="26"/>
-      <c r="F6" s="25" t="s">
-        <v>288</v>
-      </c>
+      <c r="F6" s="25"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>269</v>
-      </c>
+      <c r="J6" s="38"/>
+      <c r="K6" s="40"/>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
       <c r="B7" s="25"/>
       <c r="C7" s="4"/>
       <c r="D7" s="5"/>
       <c r="E7" s="26"/>
-      <c r="F7" s="25" t="s">
-        <v>289</v>
-      </c>
+      <c r="F7" s="25"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="29"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>277</v>
-      </c>
+      <c r="K7" s="40"/>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
       <c r="B8" s="25"/>
       <c r="C8" s="4"/>
       <c r="D8" s="5"/>
       <c r="E8" s="26"/>
-      <c r="F8" s="25" t="s">
-        <v>293</v>
-      </c>
+      <c r="F8" s="25"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="27"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>290</v>
-      </c>
+      <c r="K8" s="40"/>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
       <c r="B9" s="25"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="5" t="s">
-        <v>291</v>
-      </c>
+      <c r="D9" s="5"/>
       <c r="E9" s="26"/>
       <c r="F9" s="25"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="27"/>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>292</v>
-      </c>
+      <c r="K9" s="40"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
       <c r="B10" s="25"/>
       <c r="C10" s="4"/>
       <c r="D10" s="5"/>
       <c r="E10" s="26"/>
       <c r="F10" s="25"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="4" t="s">
-        <v>102</v>
-      </c>
+      <c r="H10" s="4"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>285</v>
-      </c>
+      <c r="J10" s="38"/>
+      <c r="K10" s="40"/>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
       <c r="B11" s="25"/>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="25" t="s">
-        <v>286</v>
-      </c>
+      <c r="F11" s="25"/>
       <c r="G11" s="5"/>
       <c r="H11" s="4"/>
       <c r="I11" s="33"/>
       <c r="J11" s="29"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>277</v>
-      </c>
+      <c r="K11" s="40"/>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
       <c r="B12" s="25"/>
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="25">
-        <v>4</v>
-      </c>
+      <c r="F12" s="25"/>
       <c r="G12" s="5"/>
       <c r="H12" s="4"/>
       <c r="I12" s="33"/>
       <c r="J12" s="27"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="40"/>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="25"/>
       <c r="C13" s="4"/>
@@ -3543,8 +3544,9 @@
       <c r="H13" s="4"/>
       <c r="I13" s="33"/>
       <c r="J13" s="27"/>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K13" s="40"/>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="25"/>
       <c r="C14" s="4"/>
@@ -3554,9 +3556,10 @@
       <c r="G14" s="5"/>
       <c r="H14" s="4"/>
       <c r="I14" s="33"/>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J14" s="38"/>
+      <c r="K14" s="40"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="25"/>
       <c r="C15" s="4"/>
@@ -3567,8 +3570,9 @@
       <c r="H15" s="4"/>
       <c r="I15" s="33"/>
       <c r="J15" s="29"/>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K15" s="40"/>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="25"/>
       <c r="C16" s="4"/>
@@ -3579,8 +3583,9 @@
       <c r="H16" s="4"/>
       <c r="I16" s="33"/>
       <c r="J16" s="27"/>
-    </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K16" s="40"/>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="25"/>
       <c r="C17" s="4"/>
@@ -3591,8 +3596,9 @@
       <c r="H17" s="4"/>
       <c r="I17" s="33"/>
       <c r="J17" s="27"/>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K17" s="40"/>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="25"/>
       <c r="C18" s="4"/>
@@ -3602,9 +3608,10 @@
       <c r="G18" s="5"/>
       <c r="H18" s="4"/>
       <c r="I18" s="33"/>
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J18" s="38"/>
+      <c r="K18" s="40"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="34"/>
       <c r="C19" s="26"/>
@@ -3615,8 +3622,9 @@
       <c r="H19" s="4"/>
       <c r="I19" s="33"/>
       <c r="J19" s="29"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="40"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="34"/>
       <c r="C20" s="26"/>
@@ -3627,8 +3635,9 @@
       <c r="H20" s="4"/>
       <c r="I20" s="33"/>
       <c r="J20" s="27"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="40"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="34"/>
       <c r="C21" s="26"/>
@@ -3639,8 +3648,9 @@
       <c r="H21" s="4"/>
       <c r="I21" s="33"/>
       <c r="J21" s="27"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="40"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="34"/>
       <c r="C22" s="26"/>
@@ -3651,8 +3661,9 @@
       <c r="H22" s="4"/>
       <c r="I22" s="33"/>
       <c r="J22" s="27"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" s="40"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="34"/>
       <c r="C23" s="26"/>
@@ -3663,8 +3674,9 @@
       <c r="H23" s="4"/>
       <c r="I23" s="33"/>
       <c r="J23" s="27"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" s="40"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="34"/>
       <c r="C24" s="26"/>
@@ -3675,8 +3687,9 @@
       <c r="H24" s="4"/>
       <c r="I24" s="33"/>
       <c r="J24" s="27"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" s="40"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="34"/>
       <c r="C25" s="26"/>
@@ -3687,8 +3700,9 @@
       <c r="H25" s="4"/>
       <c r="I25" s="33"/>
       <c r="J25" s="27"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" s="40"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="34"/>
       <c r="C26" s="26"/>
@@ -3699,33 +3713,34 @@
       <c r="H26" s="4"/>
       <c r="I26" s="33"/>
       <c r="J26" s="27"/>
+      <c r="K26" s="40"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <dataConsolidate/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="G2:G26">
-    <cfRule type="expression" dxfId="30" priority="45">
+    <cfRule type="expression" dxfId="32" priority="45">
       <formula>IF(AND(AND(A2="_cmd",D2=""),AND(A2="_cmd",E2="")),0,IF(AND(A2="_dektec",E2="_start"),0,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I26">
-    <cfRule type="expression" dxfId="29" priority="47">
+    <cfRule type="expression" dxfId="31" priority="47">
       <formula>IF(OR(AND(A2="_quantum",H2=""),AND(A2="_dektec",E2="_start")),0,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H26">
-    <cfRule type="expression" dxfId="28" priority="46">
+    <cfRule type="expression" dxfId="30" priority="46">
       <formula>IF(OR(AND(A2="_quantum",I2=""),A2="_astro",AND(A2="_dektec",E2="_start")),0,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D26">
-    <cfRule type="expression" dxfId="27" priority="3">
+    <cfRule type="expression" dxfId="29" priority="3">
       <formula>IF(AND(AND(A2="_cmd",G2=""),AND(A2="_cmd",E2="")),0,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E26">
-    <cfRule type="expression" dxfId="26" priority="8">
+    <cfRule type="expression" dxfId="28" priority="8">
       <formula>IF(AND(AND(A2="_cmd",D2=""),AND(A2="_cmd",G2="")),0,IF(AND(A2="_dektec"),0,1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3770,12 +3785,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A26">
       <formula1>RC_Key</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="lessThanOrEqual" showInputMessage="1" sqref="F3:F26">
-      <formula1>INDIRECT(A3)</formula1>
-    </dataValidation>
-    <dataValidation type="list" operator="lessThanOrEqual" showInputMessage="1" sqref="F2">
+    <dataValidation type="list" operator="lessThanOrEqual" showInputMessage="1" sqref="F2:F26">
       <formula1>INDIRECT(A2)</formula1>
     </dataValidation>
+    <dataValidation operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K26"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3787,7 +3800,7 @@
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="44" id="{C7B2E7EC-C897-41EE-B25E-2FF3E7A400FF}">
-            <xm:f>IF(OR(A2="_log1",A2="_log2",A2='Selection List'!$A$11:$A$22,A2='Selection List'!$A$24:$A$33,A2="_audio_debounce",A2="_DOS",A2="_pwm"),0,1)</xm:f>
+            <xm:f>IF(OR(A2="_log1",A2="_log2",A2='Selection List'!$A$12:$A$23,A2='Selection List'!$A$25:$A$34,A2="_audio_debounce",A2="_DOS",A2="_pwm",A2="_hex",A2="_SXP"),0,1)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -3806,10 +3819,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L114"/>
+  <dimension ref="A1:L116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3895,7 +3908,7 @@
         <v>246</v>
       </c>
       <c r="L2" t="s">
-        <v>294</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -3986,8 +3999,8 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>216</v>
+      <c r="A6" s="20" t="s">
+        <v>279</v>
       </c>
       <c r="E6" s="24" t="s">
         <v>223</v>
@@ -4014,7 +4027,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E7" s="24" t="s">
         <v>224</v>
@@ -4041,7 +4054,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="E8" s="24" t="s">
         <v>225</v>
@@ -4068,7 +4081,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E9" s="24" t="s">
         <v>226</v>
@@ -4095,7 +4108,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E10" s="24" t="s">
         <v>227</v>
@@ -4113,8 +4126,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
-        <v>256</v>
+      <c r="A11" s="19" t="s">
+        <v>233</v>
       </c>
       <c r="E11" s="24" t="s">
         <v>228</v>
@@ -4131,7 +4144,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
-        <v>234</v>
+        <v>256</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>107</v>
@@ -4145,7 +4158,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>108</v>
@@ -4159,7 +4172,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>109</v>
@@ -4170,7 +4183,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>110</v>
@@ -4181,7 +4194,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>111</v>
@@ -4192,7 +4205,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>112</v>
@@ -4203,7 +4216,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>113</v>
@@ -4214,7 +4227,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>114</v>
@@ -4225,7 +4238,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>115</v>
@@ -4236,7 +4249,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>116</v>
@@ -4247,7 +4260,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>117</v>
@@ -4257,8 +4270,8 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
-        <v>258</v>
+      <c r="A23" s="30" t="s">
+        <v>255</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>118</v>
@@ -4268,8 +4281,8 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="36" t="s">
-        <v>261</v>
+      <c r="A24" s="35" t="s">
+        <v>258</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>119</v>
@@ -4280,7 +4293,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="36" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>120</v>
@@ -4291,7 +4304,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="36" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>121</v>
@@ -4302,7 +4315,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="36" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>122</v>
@@ -4313,7 +4326,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="36" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>123</v>
@@ -4324,7 +4337,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="36" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>124</v>
@@ -4335,7 +4348,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="36" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>125</v>
@@ -4346,7 +4359,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="36" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>126</v>
@@ -4357,7 +4370,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="36" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>127</v>
@@ -4368,7 +4381,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="36" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>127</v>
@@ -4378,8 +4391,8 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="37" t="s">
-        <v>278</v>
+      <c r="A34" s="36" t="s">
+        <v>270</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>128</v>
@@ -4389,8 +4402,8 @@
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
-        <v>14</v>
+      <c r="A35" s="37" t="s">
+        <v>277</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>129</v>
@@ -4401,7 +4414,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>15</v>
+        <v>282</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>130</v>
@@ -4412,7 +4425,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>131</v>
@@ -4423,7 +4436,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>132</v>
@@ -4434,7 +4447,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>133</v>
@@ -4445,7 +4458,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>134</v>
@@ -4456,7 +4469,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F41" s="8" t="s">
         <v>135</v>
@@ -4467,7 +4480,7 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F42" s="8" t="s">
         <v>136</v>
@@ -4478,7 +4491,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F43" s="8" t="s">
         <v>137</v>
@@ -4489,7 +4502,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F44" s="8" t="s">
         <v>138</v>
@@ -4500,7 +4513,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>139</v>
@@ -4511,7 +4524,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>140</v>
@@ -4522,7 +4535,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="F47" s="8" t="s">
         <v>141</v>
@@ -4533,7 +4546,7 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="F48" s="8" t="s">
         <v>142</v>
@@ -4544,7 +4557,7 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
       <c r="F49" s="8" t="s">
         <v>143</v>
@@ -4555,7 +4568,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="F50" s="8" t="s">
         <v>144</v>
@@ -4566,7 +4579,7 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="F51" s="8" t="s">
         <v>145</v>
@@ -4577,7 +4590,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="F52" s="8" t="s">
         <v>146</v>
@@ -4588,7 +4601,7 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="F53" s="8" t="s">
         <v>147</v>
@@ -4599,7 +4612,7 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="F54" s="8" t="s">
         <v>148</v>
@@ -4610,7 +4623,7 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="F55" s="8" t="s">
         <v>149</v>
@@ -4621,7 +4634,7 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
       <c r="F56" s="8" t="s">
         <v>150</v>
@@ -4632,7 +4645,7 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F57" s="8" t="s">
         <v>151</v>
@@ -4643,7 +4656,7 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="F58" s="8" t="s">
         <v>152</v>
@@ -4654,7 +4667,7 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="F59" s="8" t="s">
         <v>153</v>
@@ -4665,7 +4678,7 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="F60" s="8" t="s">
         <v>154</v>
@@ -4676,7 +4689,7 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="F61" s="8" t="s">
         <v>155</v>
@@ -4687,7 +4700,7 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="F62" s="8" t="s">
         <v>156</v>
@@ -4698,7 +4711,7 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="F63" s="8" t="s">
         <v>157</v>
@@ -4709,7 +4722,7 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="F64" s="8" t="s">
         <v>158</v>
@@ -4720,7 +4733,7 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="F65" s="8" t="s">
         <v>159</v>
@@ -4731,7 +4744,7 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="F66" s="8" t="s">
         <v>160</v>
@@ -4742,7 +4755,7 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F67" s="8" t="s">
         <v>161</v>
@@ -4753,7 +4766,7 @@
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="F68" s="8" t="s">
         <v>162</v>
@@ -4764,7 +4777,7 @@
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F69" s="8" t="s">
         <v>163</v>
@@ -4775,7 +4788,7 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="F70" s="8" t="s">
         <v>164</v>
@@ -4786,7 +4799,7 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="F71" s="8" t="s">
         <v>165</v>
@@ -4797,7 +4810,7 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="F72" s="8" t="s">
         <v>166</v>
@@ -4808,7 +4821,7 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
       <c r="F73" s="8" t="s">
         <v>167</v>
@@ -4819,7 +4832,7 @@
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F74" s="8" t="s">
         <v>168</v>
@@ -4830,7 +4843,7 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="F75" s="8" t="s">
         <v>169</v>
@@ -4841,7 +4854,7 @@
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="F76" s="8" t="s">
         <v>170</v>
@@ -4852,7 +4865,7 @@
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F77" s="8" t="s">
         <v>171</v>
@@ -4863,7 +4876,7 @@
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="F78" s="8" t="s">
         <v>172</v>
@@ -4874,7 +4887,7 @@
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="F79" s="8" t="s">
         <v>173</v>
@@ -4885,7 +4898,7 @@
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F80" s="8" t="s">
         <v>174</v>
@@ -4896,7 +4909,7 @@
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="10" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="F81" s="8" t="s">
         <v>175</v>
@@ -4907,7 +4920,7 @@
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="F82" s="8" t="s">
         <v>176</v>
@@ -4918,7 +4931,7 @@
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="F83" s="8" t="s">
         <v>177</v>
@@ -4929,7 +4942,7 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F84" s="8" t="s">
         <v>178</v>
@@ -4940,7 +4953,7 @@
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="10" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="F85" s="8" t="s">
         <v>179</v>
@@ -4951,7 +4964,7 @@
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="10" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="F86" s="8" t="s">
         <v>180</v>
@@ -4962,7 +4975,7 @@
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="10" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F87" s="8" t="s">
         <v>181</v>
@@ -4973,7 +4986,7 @@
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="10" t="s">
-        <v>87</v>
+        <v>35</v>
       </c>
       <c r="F88" s="8" t="s">
         <v>182</v>
@@ -4984,7 +4997,7 @@
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="10" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="F89" s="8" t="s">
         <v>183</v>
@@ -4995,7 +5008,7 @@
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="10" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="F90" s="8" t="s">
         <v>184</v>
@@ -5006,7 +5019,7 @@
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="10" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="F91" s="8" t="s">
         <v>185</v>
@@ -5017,7 +5030,7 @@
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="10" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="F92" s="8" t="s">
         <v>186</v>
@@ -5028,7 +5041,7 @@
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="10" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F93" s="8" t="s">
         <v>187</v>
@@ -5039,7 +5052,7 @@
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="10" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="F94" s="8" t="s">
         <v>188</v>
@@ -5050,7 +5063,7 @@
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="10" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="F95" s="8" t="s">
         <v>189</v>
@@ -5061,7 +5074,7 @@
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="10" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="F96" s="8" t="s">
         <v>190</v>
@@ -5072,7 +5085,7 @@
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="10" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="F97" s="8" t="s">
         <v>191</v>
@@ -5083,7 +5096,7 @@
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="10" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="F98" s="8" t="s">
         <v>192</v>
@@ -5094,7 +5107,7 @@
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="10" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="F99" s="8" t="s">
         <v>193</v>
@@ -5105,7 +5118,7 @@
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="10" t="s">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="F100" s="8" t="s">
         <v>194</v>
@@ -5116,7 +5129,7 @@
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="10" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="F101" s="8" t="s">
         <v>195</v>
@@ -5127,7 +5140,7 @@
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="10" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="F102" s="8" t="s">
         <v>196</v>
@@ -5138,7 +5151,7 @@
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="10" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="F103" s="8" t="s">
         <v>197</v>
@@ -5149,7 +5162,7 @@
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="10" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="F104" s="8" t="s">
         <v>198</v>
@@ -5157,7 +5170,7 @@
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="10" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
       <c r="F105" s="8" t="s">
         <v>199</v>
@@ -5165,46 +5178,56 @@
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="10" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="10" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="10" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="10" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="10" t="s">
-        <v>88</v>
+        <v>12</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="10" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="10" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>